<commit_message>
PCB changes. Calulation price changed
</commit_message>
<xml_diff>
--- a/Doc/SubBuoyCostCalculation.xlsx
+++ b/Doc/SubBuoyCostCalculation.xlsx
@@ -318,10 +318,10 @@
   <dimension ref="A2:P1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J11" activeCellId="0" sqref="J11"/>
+      <selection pane="topLeft" activeCell="G22" activeCellId="0" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.28125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.71"/>
@@ -497,11 +497,11 @@
         <v>21</v>
       </c>
       <c r="D8" s="1" t="n">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="E8" s="1" t="n">
         <f aca="false">A8*D8</f>
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="I8" s="0" t="s">
         <v>22</v>
@@ -527,11 +527,11 @@
         <v>27</v>
       </c>
       <c r="D9" s="1" t="n">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="E9" s="1" t="n">
         <f aca="false">A9*D9</f>
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>28</v>
@@ -550,7 +550,7 @@
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E10" s="1" t="n">
         <f aca="false">SUM(E4:E9)</f>
-        <v>313</v>
+        <v>283</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>19</v>
@@ -600,11 +600,11 @@
         <v>31</v>
       </c>
       <c r="D16" s="1" t="n">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="E16" s="1" t="n">
         <f aca="false">A16*D16</f>
-        <v>50</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -618,23 +618,27 @@
         <v>27</v>
       </c>
       <c r="D17" s="1" t="n">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="E17" s="1" t="n">
         <f aca="false">A17*D17</f>
-        <v>30</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E18" s="1" t="n">
         <f aca="false">SUM(E15:E17)</f>
-        <v>95</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E20" s="1" t="n">
         <f aca="false">E10+E18</f>
-        <v>408</v>
+        <v>348</v>
+      </c>
+      <c r="G20" s="1" t="n">
+        <f aca="false">E20*3</f>
+        <v>1044</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>